<commit_message>
Open and Closed postions separated
</commit_message>
<xml_diff>
--- a/docs/Samples/Events.xlsx
+++ b/docs/Samples/Events.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>PositionClosed</t>
+  </si>
+  <si>
+    <t>Jimmy MLP</t>
+  </si>
+  <si>
+    <t>US398882994</t>
   </si>
 </sst>
 </file>
@@ -448,11 +454,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,21 +833,64 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42675</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="5">
+        <v>30</v>
+      </c>
+      <c r="F18" s="7">
+        <v>22</v>
+      </c>
+      <c r="G18" s="7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>42736</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="8">
         <v>4</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G19" s="7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3">
+        <v>42736</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="8">
+        <v>20</v>
+      </c>
+      <c r="G20" s="7">
         <v>9.9</v>
       </c>
     </row>

</xml_diff>